<commit_message>
Feat: Atualizando lista de variações de frase
</commit_message>
<xml_diff>
--- a/textos_para_fala.xlsx
+++ b/textos_para_fala.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jarvis\Documents\Parla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B36CDBE6-3AE9-4486-BED7-0DD8D0BFB70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12CC818-8850-400E-ABF4-B6AEFE39183B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DEAC8C37-1DDE-489C-B42D-B5330F9B6029}"/>
   </bookViews>
@@ -36,31 +36,273 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="81">
   <si>
     <t>Texto</t>
   </si>
   <si>
-    <t>Faça um pix de 10 para 1112131415</t>
-  </si>
-  <si>
-    <t>Faça um pix de 20 para 1112131415</t>
-  </si>
-  <si>
-    <t>Quero um pix de 1000 para Luana</t>
-  </si>
-  <si>
-    <t>Mande 50 para Isaac</t>
+    <t>Pix de 500 reais para Joaquim</t>
+  </si>
+  <si>
+    <t>Mandar 50 para o Salles</t>
+  </si>
+  <si>
+    <t>25,30 para monicagb@teste.com</t>
+  </si>
+  <si>
+    <t>300 para minhaconta68@teste.com</t>
+  </si>
+  <si>
+    <t>Enviar 100 reais para Ribeiro</t>
+  </si>
+  <si>
+    <t>300 para monicagb@teste.com</t>
+  </si>
+  <si>
+    <t>Realizar transferência de 50 para Salles</t>
+  </si>
+  <si>
+    <t>Realizar transferência de 200 para Joaquim</t>
+  </si>
+  <si>
+    <t>Transferir 300 para Ribeiro</t>
+  </si>
+  <si>
+    <t>Enviar 25,30 para o 00015578000111</t>
+  </si>
+  <si>
+    <t>Pix de 100 reais para 00015578000111</t>
+  </si>
+  <si>
+    <t>Transferir 75,50 para Carminha</t>
+  </si>
+  <si>
+    <t>Mandar 25,30 para o Joaquim</t>
+  </si>
+  <si>
+    <t>Depositar 10,00 na conta de Salles</t>
+  </si>
+  <si>
+    <t>Fazer um pix de 75,50 para Salles</t>
+  </si>
+  <si>
+    <t>Efetuar um pix de 75,50 para Salles</t>
+  </si>
+  <si>
+    <t>Transferir 35,99 para monicagb@teste.com</t>
+  </si>
+  <si>
+    <t>Mandar 10,00 para o 00015578000111</t>
+  </si>
+  <si>
+    <t>Depositar 500 na conta de 00015578000111</t>
+  </si>
+  <si>
+    <t>50 para Carminha</t>
+  </si>
+  <si>
+    <t>Envie 500 reais para o Joaquim</t>
+  </si>
+  <si>
+    <t>Mande quinhentos reais para o Joaquim</t>
+  </si>
+  <si>
+    <t>Faça um Pix de 500 reais para o Joaquim</t>
+  </si>
+  <si>
+    <t>Transfira 500 reais para o Joaquim</t>
+  </si>
+  <si>
+    <t>Envie 50 reais para o Salles</t>
+  </si>
+  <si>
+    <t>Mande cinquenta reais para o Salles</t>
+  </si>
+  <si>
+    <t>Faz um Pix de 50 reais para o Salles</t>
+  </si>
+  <si>
+    <t>Transfira 50 reais para o Salles</t>
+  </si>
+  <si>
+    <t>Envie 25,30 reais para o monicagb@teste.com</t>
+  </si>
+  <si>
+    <t>Mande 25 reais e 30 centavos para o monicagb@teste.com</t>
+  </si>
+  <si>
+    <t>Faça um Pix de 25,30 reais para o monicagb@teste.com</t>
+  </si>
+  <si>
+    <t>Transfira 25,30 reais para o monicagb@teste.com</t>
+  </si>
+  <si>
+    <t>Envie 300 reais para o minhaconta68@teste.com</t>
+  </si>
+  <si>
+    <t>Mande trezentos reais para o minhaconta68@teste.com</t>
+  </si>
+  <si>
+    <t>Faça um Pix de 300 reais para o minhaconta68@teste.com</t>
+  </si>
+  <si>
+    <t>Transfira 300 reais para o minhaconta68@teste.com</t>
+  </si>
+  <si>
+    <t>Envie 100 reais para o Ribeiro</t>
+  </si>
+  <si>
+    <t>Mande cem reais para o Ribeiro</t>
+  </si>
+  <si>
+    <t>Faz um Pix de 100 reais para o Ribeiro</t>
+  </si>
+  <si>
+    <t>Transfira 100 reais para o Ribeiro</t>
+  </si>
+  <si>
+    <t>Envie 300 reais para o monicagb@teste.com</t>
+  </si>
+  <si>
+    <t>Mande trezentos reais para o monicagb@teste.com</t>
+  </si>
+  <si>
+    <t>Faça um Pix de 300 reais para o monicagb@teste.com</t>
+  </si>
+  <si>
+    <t>Transfira 300 reais para o monicagb@teste.com</t>
+  </si>
+  <si>
+    <t>Envie 200 reais para o Joaquim</t>
+  </si>
+  <si>
+    <t>Mande duzentos reais para o Joaquim</t>
+  </si>
+  <si>
+    <t>Faça um Pix de 200 reais para o Joaquim</t>
+  </si>
+  <si>
+    <t>Transfira 200 reais para o Joaquim</t>
+  </si>
+  <si>
+    <t>Envie 75,50 reais para a Carminha</t>
+  </si>
+  <si>
+    <t>Mande setenta e cinco reais e cinquenta centavos para a Carminha</t>
+  </si>
+  <si>
+    <t>Faça um Pix de 75,50 reais para a Carminha</t>
+  </si>
+  <si>
+    <t>Transfira 75,50 reais para a Carminha</t>
+  </si>
+  <si>
+    <t>Envie 25,30 reais para o Joaquim</t>
+  </si>
+  <si>
+    <t>Mande 25 reais e 30 centavos para o Joaquim</t>
+  </si>
+  <si>
+    <t>Faça um Pix de 25,30 reais para o Joaquim</t>
+  </si>
+  <si>
+    <t>Transfira 25,30 reais para o Joaquim</t>
+  </si>
+  <si>
+    <t>Envie 10 reais para o Salles</t>
+  </si>
+  <si>
+    <t>Mande dez reais para o Salles</t>
+  </si>
+  <si>
+    <t>Faz um Pix de 10 reais para o Salles</t>
+  </si>
+  <si>
+    <t>Transfira 10 reais para o Salles</t>
+  </si>
+  <si>
+    <t>Envie 75,50 reais para o Salles</t>
+  </si>
+  <si>
+    <t>Mande setenta e cinco reais e cinquenta centavos para o Salles</t>
+  </si>
+  <si>
+    <t>Faça um Pix de 75,50 reais para o Salles</t>
+  </si>
+  <si>
+    <t>Transfira 75,50 reais para o Salles</t>
+  </si>
+  <si>
+    <t>Envie 35,99 reais para o monicagb@teste.com</t>
+  </si>
+  <si>
+    <t>Mande trinta e cinco reais e noventa e nove centavos para o monicagb@teste.com</t>
+  </si>
+  <si>
+    <t>Faça um Pix de 35,99 reais para o monicagb@teste.com</t>
+  </si>
+  <si>
+    <t>Transfira 35,99 reais para o monicagb@teste.com</t>
+  </si>
+  <si>
+    <t>Envie 10 reais para o 00015578000111</t>
+  </si>
+  <si>
+    <t>Mande dez reais para o 00015578000111</t>
+  </si>
+  <si>
+    <t>Faz um Pix de 10 reais para o 00015578000111</t>
+  </si>
+  <si>
+    <t>Transfira 10 reais para o 00015578000111</t>
+  </si>
+  <si>
+    <t>Envie 500 reais para o 00015578000111</t>
+  </si>
+  <si>
+    <t>Mande quinhentos reais para o 00015578000111</t>
+  </si>
+  <si>
+    <t>Faça um Pix de 500 reais para o 00015578000111</t>
+  </si>
+  <si>
+    <t>Transfira 500 reais para o 00015578000111</t>
+  </si>
+  <si>
+    <t>Envie 50 reais para a Carminha</t>
+  </si>
+  <si>
+    <t>Mande cinquenta reais para a Carminha</t>
+  </si>
+  <si>
+    <t>Faz um Pix de 50 reais para a Carminha</t>
+  </si>
+  <si>
+    <t>Transfira 50 reais para a Carminha</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -83,13 +325,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -422,15 +672,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2342C126-692A-4B57-8471-3A528AACC9B4}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="74.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -439,26 +689,432 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" tooltip="mailto:monicagb@teste.com" display="mailto:monicagb@teste.com" xr:uid="{756A5766-E7FE-42ED-B578-A2BE53B54477}"/>
+    <hyperlink ref="A5" r:id="rId2" tooltip="mailto:minhaconta68@teste.com" display="mailto:minhaconta68@teste.com" xr:uid="{555CB9EA-8EDC-4001-9DC5-3EA28221DA86}"/>
+    <hyperlink ref="A7" r:id="rId3" tooltip="mailto:monicagb@teste.com" display="mailto:monicagb@teste.com" xr:uid="{3E7E83DE-7D6E-4AD2-A1CA-B5000B2EB0DB}"/>
+    <hyperlink ref="A18" r:id="rId4" tooltip="mailto:monicagb@teste.com" display="mailto:monicagb@teste.com" xr:uid="{0641E423-FADA-45C4-874F-8E28E952844B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>